<commit_message>
webapp for company group
started working on the web app
</commit_message>
<xml_diff>
--- a/CompanyGroup/testing/Information_on_company_group.xlsx
+++ b/CompanyGroup/testing/Information_on_company_group.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -37,113 +37,225 @@
     <t>Paid up capital</t>
   </si>
   <si>
-    <t>E.I.D PARRY (INDIA) LIMITED</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>EID PARRYS LTD,,
-WARE HOUSE,PB. NO.:2,CHENNAI685TN
-CHENNAI-600001</t>
-  </si>
-  <si>
-    <t>22 Sep 1975</t>
+    <t>MOBAR INDIA LIMITED</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Unavailable</t>
+  </si>
+  <si>
+    <t>08 Feb 1996</t>
   </si>
   <si>
     <t>Active</t>
   </si>
   <si>
-    <t>Manufacture of other chemical products</t>
-  </si>
-  <si>
-    <t>₹177,102,384</t>
-  </si>
-  <si>
-    <t>MURUGAPPA MANAGEMENT SERVICES LIMITED</t>
-  </si>
-  <si>
-    <t>MURUGAPPA MANAGEMENT SERVICES LTD.,
-NEW NO 2,N.S.C.BOSE ROAD,PARRYSCHENNAI685TN
-CHENNAI-600001</t>
-  </si>
-  <si>
-    <t>10 Jul 1972</t>
-  </si>
-  <si>
-    <t>Legal, accounting, book-keeping and auditing activities; tax consultancy; market research and public opinion polling; business and management consultancy</t>
-  </si>
-  <si>
-    <t>₹22,946,800</t>
-  </si>
-  <si>
-    <t>MURUGAPPA HOLDINGS LIMITED</t>
-  </si>
-  <si>
-    <t>Unavailable</t>
-  </si>
-  <si>
-    <t>24 Sep 1977</t>
+    <t>Other land transport</t>
+  </si>
+  <si>
+    <t>₹28,858,870</t>
+  </si>
+  <si>
+    <t>BONAI INDUSTRIAL CO LTD</t>
+  </si>
+  <si>
+    <t>Cuttack</t>
+  </si>
+  <si>
+    <t>06 Oct 1939</t>
+  </si>
+  <si>
+    <t>Quarrying of stone, sand and clay</t>
+  </si>
+  <si>
+    <t>₹76,692,800</t>
+  </si>
+  <si>
+    <t>SKILL COUNCIL FOR MINING SECTOR</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>06 Dec 2013</t>
+  </si>
+  <si>
+    <t>Mining and quarrying , n.e.c.</t>
+  </si>
+  <si>
+    <t>₹100,000</t>
+  </si>
+  <si>
+    <t>MINERALS &amp; METALS LTD</t>
+  </si>
+  <si>
+    <t>18 Dec 1940</t>
+  </si>
+  <si>
+    <t>Other financial intermediation. [This group includes financial intermediation other than that conducted by monetary institutions.]</t>
+  </si>
+  <si>
+    <t>₹606,000</t>
+  </si>
+  <si>
+    <t>ORISSA SECURITIES LTD</t>
+  </si>
+  <si>
+    <t>04 Feb 1993</t>
+  </si>
+  <si>
+    <t>Real estate activities with own or leased property. [This class includes buying, selling, renting and operating of self-owned or leased real estate such as apartment building and dwellings, non-residential buildings, developing and subdividing real estate into lots etc. Also included are development and sale of land and cemetery lots, operating of apartment hotels and residential mobile home sites.(Development on own account involving construction is classified in class 4520).]</t>
+  </si>
+  <si>
+    <t>₹10,000,000</t>
+  </si>
+  <si>
+    <t>RADHIKAPUR (WEST) COAL MINING PRIVATELIMITED</t>
+  </si>
+  <si>
+    <t>29 Mar 2010</t>
+  </si>
+  <si>
+    <t>Mining and agglomeration of hard coal [Includes under ground or open-cut mining of anthracite, bituminous or other hard coal; cleaning, sizing, pulverizing and other operations to improve the quality; operations to recover hard coal from culm banks; manufacture of briquettes or other solid fuels consisting chiefly of hard coal and in-situ gasification of coal.]</t>
+  </si>
+  <si>
+    <t>₹500,000,000</t>
+  </si>
+  <si>
+    <t>EZMA FOUNDATION</t>
+  </si>
+  <si>
+    <t>16 Dec 2009</t>
+  </si>
+  <si>
+    <t>Human health activities</t>
+  </si>
+  <si>
+    <t>₹0</t>
+  </si>
+  <si>
+    <t>ELECTROCHEM ORISSA LTD</t>
+  </si>
+  <si>
+    <t>12 Jan 1978</t>
+  </si>
+  <si>
+    <t>Manufacture of basic chemicals</t>
+  </si>
+  <si>
+    <t>₹2,764,410</t>
+  </si>
+  <si>
+    <t>FEEGRADE &amp; CO PVT LTD</t>
+  </si>
+  <si>
+    <t>14 Sep 1964</t>
+  </si>
+  <si>
+    <t>Mining and agglomeration of lignite [Includes under ground or open-cut mining of lignite (brown coal); cleaning, sizing, pulverizing and other operations to improve the quality; and manufacture of briquettes or other solid fuels consisting chiefly of lignite.]</t>
+  </si>
+  <si>
+    <t>₹44,982,000</t>
+  </si>
+  <si>
+    <t>MANGILALL ESTATES PVT LTD</t>
+  </si>
+  <si>
+    <t>28 Jun 1951</t>
+  </si>
+  <si>
+    <t>₹45,127,600</t>
+  </si>
+  <si>
+    <t>RUNGTA SONS PVT LTD</t>
+  </si>
+  <si>
+    <t>04 Mar 1943</t>
+  </si>
+  <si>
+    <t>Forestry, logging and related service activities</t>
+  </si>
+  <si>
+    <t>₹2,458</t>
+  </si>
+  <si>
+    <t>SHYAM SUNDAR LTD</t>
+  </si>
+  <si>
+    <t>29 Jun 1951</t>
+  </si>
+  <si>
+    <t>Other wholesale [Includes specialized wholesale not covered in any one of the previous categories and wholesale in a variety of goods without any particular specialization.]</t>
+  </si>
+  <si>
+    <t>₹27,533,750</t>
+  </si>
+  <si>
+    <t>C T MINING PRIVATE LIMITED</t>
+  </si>
+  <si>
+    <t>Jharkhand</t>
+  </si>
+  <si>
+    <t>25 Sep 2008</t>
+  </si>
+  <si>
+    <t>₹100,000,000</t>
+  </si>
+  <si>
+    <t>MEDNIRAI COAL MINING PRIVATE LIMITED</t>
+  </si>
+  <si>
+    <t>01 Sep 2009</t>
+  </si>
+  <si>
+    <t>₹27,000,000</t>
+  </si>
+  <si>
+    <t>BANSPANI IRON LTD</t>
+  </si>
+  <si>
+    <t>BANSPANI IRON LIMITED,
+AT/PO: BANEIKALAVIA: JODAJODAKEONJHAR
+KEONJHAR-758038</t>
+  </si>
+  <si>
+    <t>16 Sep 1994</t>
+  </si>
+  <si>
+    <t>Wholesale of non-agricultural intermediate products, waste and scrap</t>
+  </si>
+  <si>
+    <t>₹27,007,000</t>
+  </si>
+  <si>
+    <t>JP CEMENTS LIMITED</t>
+  </si>
+  <si>
+    <t>Shillong</t>
+  </si>
+  <si>
+    <t>15 Jan 2008</t>
   </si>
   <si>
     <t>Amalgamated</t>
   </si>
   <si>
-    <t>Other financial intermediation. [This group includes financial intermediation other than that conducted by monetary institutions.]</t>
-  </si>
-  <si>
-    <t>₹40,758,160</t>
-  </si>
-  <si>
-    <t>PARRY AGRO INDUSTRIES LIMITED</t>
-  </si>
-  <si>
-    <t>PARRY AGRO INDUSTRIES  LTD,,
-26/1847, BRISTOW ROADW/ISLANDKOCHI676KL
-KOCHI-682003</t>
-  </si>
-  <si>
-    <t>23 Mar 2011</t>
-  </si>
-  <si>
-    <t>Growing of crops; market gardening; horticulture</t>
-  </si>
-  <si>
-    <t>₹37,568,160</t>
-  </si>
-  <si>
-    <t>AMBADI ENTERPRISES LIMITED</t>
-  </si>
-  <si>
-    <t>AMBADI ENTERPRISES LTD.,
-DYE HOUSE DIVISION,CH-13/180CHOVVAKANNUR670KL
-KANNUR-670006</t>
-  </si>
-  <si>
-    <t>18 Nov 1941</t>
-  </si>
-  <si>
-    <t>₹4,800,000</t>
-  </si>
-  <si>
-    <t>COROMANDEL INTERNATIONAL LIMITED</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>COROMANDEL INTERNATIONAL LIMITED,
-71/72-A/72/73/74/75/83,G.I.D.CNANDESARIVADODARA566GJ
-VADODARA-391340</t>
-  </si>
-  <si>
-    <t>16 Oct 1961</t>
-  </si>
-  <si>
-    <t>Manufacture of basic chemicals</t>
-  </si>
-  <si>
-    <t>₹293,434,176</t>
+    <t>Manufacture of non-metallic mineral products n.e.c.</t>
+  </si>
+  <si>
+    <t>₹500,000</t>
+  </si>
+  <si>
+    <t>KB CEMENTS PRIVATE LIMITED</t>
+  </si>
+  <si>
+    <t>22 Mar 2007</t>
+  </si>
+  <si>
+    <t>₹150,000</t>
   </si>
 </sst>
 </file>
@@ -475,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -532,10 +644,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -555,91 +667,344 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="G7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>